<commit_message>
Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/download/TimeSheet.xlsx
+++ b/download/TimeSheet.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chenk\Desktop\kaixi\download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KaiXi\Desktop\kaixi\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B6D000-6AC5-4F9E-AF80-1E3E14A1208F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF96B7B-11FA-4866-8CCB-8FBC4D2C7251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="July" sheetId="1" r:id="rId1"/>
+    <sheet name="August" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="10">
   <si>
     <t>合計</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -68,13 +69,21 @@
     <t>165:35</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>140:20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="179" formatCode="mm\-dd;@"/>
+    <numFmt numFmtId="176" formatCode="mm\-dd;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -107,7 +116,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,6 +126,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -320,22 +335,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -345,9 +360,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -627,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -722,7 +754,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E7" s="8">
-        <f t="shared" ref="E5:E34" si="0">C7-D7-B7</f>
+        <f t="shared" ref="E7:E32" si="0">C7-D7-B7</f>
         <v>0.36458333333333337</v>
       </c>
     </row>
@@ -1115,6 +1147,535 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E35" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91DDCCDD-2138-4B81-9CA3-E2CEE6B9294E}">
+  <dimension ref="A1:E34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="19">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="13">
+        <v>44774</v>
+      </c>
+      <c r="B4" s="22">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C4" s="22">
+        <v>0.75</v>
+      </c>
+      <c r="D4" s="22">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E4" s="23">
+        <f>C4-B4-D4</f>
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="13">
+        <v>44775</v>
+      </c>
+      <c r="B5" s="22">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="C5" s="22">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D5" s="22">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E5" s="23">
+        <f>C5-B5-D5</f>
+        <v>0.35069444444444442</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="13">
+        <v>44776</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="13">
+        <v>44777</v>
+      </c>
+      <c r="B7" s="22">
+        <v>0.375</v>
+      </c>
+      <c r="C7" s="22">
+        <v>0.8125</v>
+      </c>
+      <c r="D7" s="22">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E7" s="23">
+        <f>C7-B7-D7</f>
+        <v>0.39583333333333331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="13">
+        <v>44778</v>
+      </c>
+      <c r="B8" s="22">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C8" s="22">
+        <v>0.87152777777777779</v>
+      </c>
+      <c r="D8" s="22">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E8" s="23">
+        <f>C8-B8-D8</f>
+        <v>0.43402777777777779</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="27">
+        <v>44779</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="27">
+        <v>44780</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="29"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="13">
+        <v>44781</v>
+      </c>
+      <c r="B11" s="22">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C11" s="22">
+        <v>0.625</v>
+      </c>
+      <c r="D11" s="22">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E11" s="23">
+        <f>C11-B11-D11</f>
+        <v>0.18750000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="13">
+        <v>44782</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="13">
+        <v>44783</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="27">
+        <v>44784</v>
+      </c>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="29"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="13">
+        <v>44785</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="27">
+        <v>44786</v>
+      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="29"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="27">
+        <v>44787</v>
+      </c>
+      <c r="B17" s="28">
+        <v>0.375</v>
+      </c>
+      <c r="C17" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="D17" s="28">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E17" s="29"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="13">
+        <v>44788</v>
+      </c>
+      <c r="B18" s="22">
+        <v>0.375</v>
+      </c>
+      <c r="C18" s="22">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D18" s="22">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E18" s="23">
+        <f t="shared" ref="E18:E22" si="0">C18-B18-D18</f>
+        <v>0.31249999999999994</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="13">
+        <v>44789</v>
+      </c>
+      <c r="B19" s="22">
+        <v>0.375</v>
+      </c>
+      <c r="C19" s="22">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D19" s="22">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.31249999999999994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="13">
+        <v>44790</v>
+      </c>
+      <c r="B20" s="22">
+        <v>0.375</v>
+      </c>
+      <c r="C20" s="22">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D20" s="22">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E20" s="23">
+        <f t="shared" si="0"/>
+        <v>0.35416666666666669</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="13">
+        <v>44791</v>
+      </c>
+      <c r="B21" s="22">
+        <v>0.375</v>
+      </c>
+      <c r="C21" s="22">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D21" s="22">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E21" s="23">
+        <f t="shared" si="0"/>
+        <v>0.31249999999999994</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="13">
+        <v>44792</v>
+      </c>
+      <c r="B22" s="22">
+        <v>0.375</v>
+      </c>
+      <c r="C22" s="22">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D22" s="22">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E22" s="23">
+        <f t="shared" si="0"/>
+        <v>0.31249999999999994</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="27">
+        <v>44793</v>
+      </c>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="29"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="27">
+        <v>44794</v>
+      </c>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="29"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="13">
+        <v>44795</v>
+      </c>
+      <c r="B25" s="22">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="C25" s="22">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D25" s="22">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E25" s="23">
+        <f>C25-B25-D25</f>
+        <v>0.34027777777777779</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="13">
+        <v>44796</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="13">
+        <v>44797</v>
+      </c>
+      <c r="B27" s="22">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C27" s="22">
+        <v>0.8125</v>
+      </c>
+      <c r="D27" s="22">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E27" s="23">
+        <f t="shared" ref="E27:E29" si="1">C27-B27-D27</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="13">
+        <v>44798</v>
+      </c>
+      <c r="B28" s="22">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="C28" s="22">
+        <v>0.75</v>
+      </c>
+      <c r="D28" s="22">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E28" s="23">
+        <f t="shared" si="1"/>
+        <v>0.32291666666666663</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="13">
+        <v>44799</v>
+      </c>
+      <c r="B29" s="22">
+        <v>0.375</v>
+      </c>
+      <c r="C29" s="22">
+        <v>0.75</v>
+      </c>
+      <c r="D29" s="22">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E29" s="23">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="27">
+        <v>44800</v>
+      </c>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="29"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="27">
+        <v>44801</v>
+      </c>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="29"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="13">
+        <v>44802</v>
+      </c>
+      <c r="B32" s="22">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="C32" s="22">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D32" s="22">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E32" s="23">
+        <f t="shared" ref="E32:E34" si="2">C32-B32-D32</f>
+        <v>0.29861111111111105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="13">
+        <v>44803</v>
+      </c>
+      <c r="B33" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="C33" s="22">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D33" s="22">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E33" s="23">
+        <f t="shared" si="2"/>
+        <v>0.22916666666666671</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="24">
+        <v>44804</v>
+      </c>
+      <c r="B34" s="25">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="C34" s="25">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="D34" s="25">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E34" s="26">
+        <f t="shared" si="2"/>
+        <v>0.32986111111111105</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>